<commit_message>
Datos Diarios Vacunacion Chile
</commit_message>
<xml_diff>
--- a/Hospitales/CamasHospital_Diario.xlsx
+++ b/Hospitales/CamasHospital_Diario.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1849"/>
+  <dimension ref="A1:C1853"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28103,6 +28103,66 @@
         <v>1878</v>
       </c>
     </row>
+    <row r="1850">
+      <c r="A1850" t="inlineStr">
+        <is>
+          <t>Basica</t>
+        </is>
+      </c>
+      <c r="B1850" t="inlineStr">
+        <is>
+          <t>2021-07-22</t>
+        </is>
+      </c>
+      <c r="C1850" t="n">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="B1851" t="inlineStr">
+        <is>
+          <t>2021-07-22</t>
+        </is>
+      </c>
+      <c r="C1851" t="n">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" t="inlineStr">
+        <is>
+          <t>UTI</t>
+        </is>
+      </c>
+      <c r="B1852" t="inlineStr">
+        <is>
+          <t>2021-07-22</t>
+        </is>
+      </c>
+      <c r="C1852" t="n">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="1853">
+      <c r="A1853" t="inlineStr">
+        <is>
+          <t>UCI</t>
+        </is>
+      </c>
+      <c r="B1853" t="inlineStr">
+        <is>
+          <t>2021-07-22</t>
+        </is>
+      </c>
+      <c r="C1853" t="n">
+        <v>1845</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>